<commit_message>
Updated README and added excel template
</commit_message>
<xml_diff>
--- a/files/email_list.xlsx
+++ b/files/email_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angullia/FarhanRepository/CodeCommit-Farhan-Repositories/ChimeChatroomTool/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angullia/FarhanRepository/CodeCommit-Farhan-Repositories/ChimeRoomTool/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11409B39-A150-F34C-9A52-565F61314C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB62A6-A482-F548-8E8A-4D5B6CE57915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>xxx@email.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,13 +63,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,9 +394,21 @@
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{8A4CE575-7350-3142-BD0D-FD6E13B6FCC7}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{D984EEC3-7516-2A45-A97A-F3A55E3ACC6E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>